<commit_message>
Loaded routes from excel and user interaction for desired route.
</commit_message>
<xml_diff>
--- a/src/main/resources/routes/route_SLG_NJP.xlsx
+++ b/src/main/resources/routes/route_SLG_NJP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Where-is-My-Bus\src\main\resources\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD37233-3704-4A79-A476-47B2FEB2D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063A40C6-95DF-4D34-A18E-6CAA4D4388CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9B2DE434-A901-4F98-B7F5-6EF278C78553}"/>
   </bookViews>
@@ -56,19 +56,19 @@
     <t>slack_min</t>
   </si>
   <si>
-    <t>Siliguri Junction</t>
-  </si>
-  <si>
-    <t>Sevoke More</t>
-  </si>
-  <si>
-    <t>Bidhan Market</t>
-  </si>
-  <si>
-    <t>Pradhan Nagar</t>
-  </si>
-  <si>
-    <t>NJP Station</t>
+    <t>Alipurduar</t>
+  </si>
+  <si>
+    <t>Alipurduar Chowpathy</t>
+  </si>
+  <si>
+    <t>Alipurduar Birpara</t>
+  </si>
+  <si>
+    <t>Sonapur</t>
+  </si>
+  <si>
+    <t>Falakata</t>
   </si>
 </sst>
 </file>
@@ -460,16 +460,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFA846E-AF74-4D78-853E-D80B225ED6A5}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13.109375" customWidth="1"/>
   </cols>
@@ -502,10 +504,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="4">
-        <v>26.7271</v>
+        <v>26.479900000000001</v>
       </c>
       <c r="D2" s="4">
-        <v>88.395300000000006</v>
+        <v>89.535499999999999</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -522,13 +524,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="4">
-        <v>26.740300000000001</v>
+        <v>26.480830000000001</v>
       </c>
       <c r="D3" s="4">
-        <v>88.415099999999995</v>
+        <v>89.525999999999996</v>
       </c>
       <c r="E3" s="4">
-        <v>3.2</v>
+        <v>1.5</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -542,13 +544,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="4">
-        <v>26.724599999999999</v>
+        <v>26.482810000000001</v>
       </c>
       <c r="D4" s="4">
-        <v>88.402900000000002</v>
+        <v>89.508970000000005</v>
       </c>
       <c r="E4" s="4">
-        <v>5.0999999999999996</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F4" s="4">
         <v>3</v>
@@ -562,13 +564,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="4">
-        <v>26.707899999999999</v>
+        <v>26.494</v>
       </c>
       <c r="D5" s="4">
-        <v>88.404700000000005</v>
+        <v>89.367999999999995</v>
       </c>
       <c r="E5" s="4">
-        <v>7.4</v>
+        <v>10.5</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -582,17 +584,21 @@
         <v>10</v>
       </c>
       <c r="C6" s="4">
-        <v>26.681000000000001</v>
+        <v>26.519300000000001</v>
       </c>
       <c r="D6" s="4">
-        <v>88.431600000000003</v>
+        <v>89.201999999999998</v>
       </c>
       <c r="E6" s="4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
       </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PLaced marker on map for the route with estimated distance.
</commit_message>
<xml_diff>
--- a/src/main/resources/routes/route_SLG_NJP.xlsx
+++ b/src/main/resources/routes/route_SLG_NJP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Where-is-My-Bus\src\main\resources\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063A40C6-95DF-4D34-A18E-6CAA4D4388CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664BE305-2B76-4495-8CE2-98560135D195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9B2DE434-A901-4F98-B7F5-6EF278C78553}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>stop_order</t>
   </si>
@@ -69,13 +69,49 @@
   </si>
   <si>
     <t>Falakata</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Falakata Toll</t>
+  </si>
+  <si>
+    <t>Shoni Maharaj Mandir</t>
+  </si>
+  <si>
+    <t>Torsha Dhaba</t>
+  </si>
+  <si>
+    <t>Torsha Bridge</t>
+  </si>
+  <si>
+    <t>Shilbari High School</t>
+  </si>
+  <si>
+    <t>Putimari More</t>
+  </si>
+  <si>
+    <t>Mejbil Bus Stand</t>
+  </si>
+  <si>
+    <t>Sishagore Market</t>
+  </si>
+  <si>
+    <t>Balurghat</t>
+  </si>
+  <si>
+    <t>Assam More</t>
+  </si>
+  <si>
+    <t>Signboard Market</t>
+  </si>
+  <si>
+    <t>Dhaba Shila Bristi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +126,10 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -125,6 +165,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFA846E-AF74-4D78-853E-D80B225ED6A5}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.88671875" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
@@ -476,7 +519,7 @@
     <col min="6" max="6" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -496,7 +539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -516,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -536,7 +579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -556,7 +599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -576,29 +619,269 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4">
+        <v>26.49879</v>
+      </c>
+      <c r="D6" s="4">
+        <v>89.358599999999996</v>
+      </c>
+      <c r="E6" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4">
+        <v>26.499770000000002</v>
+      </c>
+      <c r="D7" s="4">
+        <v>89.345960000000005</v>
+      </c>
+      <c r="E7" s="4">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4">
+        <v>26.501200000000001</v>
+      </c>
+      <c r="D8" s="4">
+        <v>89.330500000000001</v>
+      </c>
+      <c r="E8" s="4">
+        <v>12.7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4">
+        <v>26.501629999999999</v>
+      </c>
+      <c r="D9" s="4">
+        <v>89.326539999999994</v>
+      </c>
+      <c r="E9" s="4">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4">
+        <v>26.500800000000002</v>
+      </c>
+      <c r="D10" s="4">
+        <v>89.304320000000004</v>
+      </c>
+      <c r="E10" s="4">
+        <v>13.2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="C6" s="4">
-        <v>26.519300000000001</v>
-      </c>
-      <c r="D6" s="4">
-        <v>89.201999999999998</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4">
+        <v>26.501049999999999</v>
+      </c>
+      <c r="D11" s="4">
+        <v>89.294700000000006</v>
+      </c>
+      <c r="E11" s="4">
+        <v>13.5</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4">
+        <v>26.501169999999998</v>
+      </c>
+      <c r="D12" s="4">
+        <v>89.287850000000006</v>
+      </c>
+      <c r="E12" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="4">
+        <v>26.50723</v>
+      </c>
+      <c r="D13" s="4">
+        <v>89.271960000000007</v>
+      </c>
+      <c r="E13" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4">
+        <v>26.511230000000001</v>
+      </c>
+      <c r="D14" s="4">
+        <v>89.261420000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>14.3</v>
+      </c>
+      <c r="F14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4">
+        <v>26.509599999999999</v>
+      </c>
+      <c r="D15" s="4">
+        <v>89.254729999999995</v>
+      </c>
+      <c r="E15" s="4">
+        <v>14.5</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="F6" s="4">
+      <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4">
+        <v>26.508710000000001</v>
+      </c>
+      <c r="D16" s="4">
+        <v>89.238929999999996</v>
+      </c>
+      <c r="E16" s="4">
+        <v>14.7</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4">
+        <v>26.513500000000001</v>
+      </c>
+      <c r="D17" s="4">
+        <v>89.218699999999998</v>
+      </c>
+      <c r="E17" s="4">
+        <v>14.8</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="4">
+        <v>26.517209999999999</v>
+      </c>
+      <c r="D18" s="4">
+        <v>89.206940000000003</v>
+      </c>
+      <c r="E18" s="4">
+        <v>15</v>
+      </c>
+      <c r="F18" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="4"/>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1"/>
+      <c r="B19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>